<commit_message>
Saud && Abdulla updated burndown chart
</commit_message>
<xml_diff>
--- a/Documentation/Burndown Chart Sprint 5.xlsx
+++ b/Documentation/Burndown Chart Sprint 5.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Student Allocated</t>
   </si>
@@ -51,10 +51,13 @@
     <t>Complete UI / examples of pdf's</t>
   </si>
   <si>
-    <t>Complete UI / Sql forms</t>
+    <t>Complete UI / Patient history form and patient activties</t>
   </si>
   <si>
-    <t>Assist completing UI/ Sql to back all the forms</t>
+    <t>Complete UI / Medical techincation form and Faniancial fees form</t>
+  </si>
+  <si>
+    <t>Assist completing UI / Sql to back all the forms</t>
   </si>
 </sst>
 </file>
@@ -255,11 +258,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -296,11 +298,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -327,32 +328,28 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Assist completing UI/ Sql to back all the forms</c:v>
+                  <c:v>Assist completing UI / Sql to back all the forms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -369,9 +366,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -397,11 +396,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -527,32 +526,28 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Complete UI / Sql forms</c:v>
+                  <c:v>Complete UI / Medical techincation form and Faniancial fees form</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -569,9 +564,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -597,11 +594,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -672,40 +669,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -733,26 +730,22 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -769,9 +762,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -797,11 +792,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -927,32 +922,28 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Complete UI / examples of pdf's</c:v>
+                  <c:v>Complete UI / Patient history form and patient activties</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -969,9 +960,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -997,11 +990,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1072,46 +1065,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,26 +1123,22 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -1169,9 +1155,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1197,11 +1185,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1333,26 +1321,22 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:spPr>
@@ -1369,9 +1353,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1397,11 +1383,11 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -1469,43 +1455,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1524,45 +1510,62 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1122567024"/>
-        <c:axId val="-1122566480"/>
+        <c:axId val="-1516858240"/>
+        <c:axId val="-1516871296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1122567024"/>
+        <c:axId val="-1516858240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1573,7 +1576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1122566480"/>
+        <c:crossAx val="-1516871296"/>
         <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,11 +1586,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1122566480"/>
+        <c:axId val="-1516871296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1596,15 +1599,14 @@
                 <a:gsLst>
                   <a:gs pos="100000">
                     <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:gs>
                 </a:gsLst>
@@ -1624,9 +1626,8 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1657,9 +1658,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1675,7 +1675,33 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1122567024"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1516858240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1688,7 +1714,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:legendEntry>
         <c:idx val="0"/>
         <c:txPr>
@@ -1698,9 +1724,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1721,9 +1746,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1744,9 +1768,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1767,9 +1790,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1790,9 +1812,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1813,9 +1834,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1830,12 +1850,7 @@
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1848,9 +1863,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1867,30 +1881,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -1956,15 +1957,14 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" b="1" kern="1200"/>
@@ -1974,23 +1974,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -2000,30 +1988,17 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2033,120 +2008,156 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
           <a:lumMod val="65000"/>
           <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
         </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2170,17 +2181,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2192,7 +2202,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2204,10 +2214,10 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2221,12 +2231,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2240,9 +2249,8 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2270,15 +2278,14 @@
           <a:gsLst>
             <a:gs pos="100000">
               <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -2296,25 +2303,27 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="100000">
               <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2328,12 +2337,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2347,11 +2355,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2360,19 +2368,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea>
@@ -2396,22 +2395,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2424,9 +2411,8 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2438,12 +2424,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2452,12 +2437,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -2467,9 +2454,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2483,15 +2469,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2500,16 +2488,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2533,8 +2515,8 @@
       <xdr:rowOff>6985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>363855</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>312566</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>138430</xdr:rowOff>
     </xdr:to>
@@ -2889,13 +2871,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16"/>
     <col min="3" max="1025" width="8.5703125"/>
   </cols>
@@ -2970,7 +2952,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -3020,46 +3002,46 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
@@ -3120,53 +3102,51 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -3225,55 +3205,55 @@
       <c r="B8" s="5"/>
       <c r="C8" s="1">
         <f t="shared" ref="C8" si="0">SUM(C3:C7)</f>
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ref="D8" si="1">SUM(D3:D7)</f>
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:P8" si="2">SUM(E3:E7)</f>
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="O8" s="1">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="2"/>

</xml_diff>